<commit_message>
sua file cau hoi Ly11.xlsx
</commit_message>
<xml_diff>
--- a/Ly11.xlsx
+++ b/Ly11.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\LTUDQL1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\LTUDQL1\DA-LTUDQL1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -70,9 +70,6 @@
     <t>GoiY</t>
   </si>
   <si>
-    <t>K10</t>
-  </si>
-  <si>
     <t>Lý thuyết chương 3</t>
   </si>
   <si>
@@ -797,18 +794,28 @@
   <si>
     <t>Lý thuyết chương 6</t>
   </si>
+  <si>
+    <t>K11</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -858,14 +865,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1175,7 +1182,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E3" sqref="E3:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,7 +1218,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1220,10 +1227,10 @@
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F2" t="s">
         <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1231,7 +1238,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1240,10 +1247,10 @@
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" t="s">
         <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1251,7 +1258,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1260,10 +1267,10 @@
         <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>141</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1271,7 +1278,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1280,10 +1287,10 @@
         <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
+        <v>141</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1291,7 +1298,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1300,10 +1307,10 @@
         <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>13</v>
+        <v>141</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1311,7 +1318,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1320,10 +1327,10 @@
         <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>13</v>
+        <v>141</v>
       </c>
       <c r="F7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1331,7 +1338,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1340,10 +1347,10 @@
         <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>13</v>
+        <v>141</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1351,7 +1358,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -1360,10 +1367,10 @@
         <v>10</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>13</v>
+        <v>141</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1371,7 +1378,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -1380,10 +1387,10 @@
         <v>10</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>13</v>
+        <v>141</v>
       </c>
       <c r="F10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1391,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -1400,10 +1407,10 @@
         <v>10</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>13</v>
+        <v>141</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1411,7 +1418,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -1420,10 +1427,10 @@
         <v>10</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>13</v>
+        <v>141</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1431,7 +1438,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -1440,10 +1447,10 @@
         <v>10</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>13</v>
+        <v>141</v>
       </c>
       <c r="F13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
@@ -1451,7 +1458,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -1460,10 +1467,10 @@
         <v>10</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>13</v>
+        <v>141</v>
       </c>
       <c r="F14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
@@ -1471,7 +1478,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C15">
         <v>3</v>
@@ -1480,10 +1487,10 @@
         <v>10</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>13</v>
+        <v>141</v>
       </c>
       <c r="F15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1491,7 +1498,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16">
         <v>3</v>
@@ -1500,10 +1507,10 @@
         <v>10</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>13</v>
+        <v>141</v>
       </c>
       <c r="F16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1511,7 +1518,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17">
         <v>3</v>
@@ -1520,10 +1527,10 @@
         <v>10</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>13</v>
+        <v>141</v>
       </c>
       <c r="F17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1531,7 +1538,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18">
         <v>3</v>
@@ -1540,10 +1547,10 @@
         <v>10</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>13</v>
+        <v>141</v>
       </c>
       <c r="F18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
@@ -1551,7 +1558,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19">
         <v>3</v>
@@ -1560,10 +1567,10 @@
         <v>10</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>13</v>
+        <v>141</v>
       </c>
       <c r="F19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1571,7 +1578,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20">
         <v>3</v>
@@ -1580,10 +1587,10 @@
         <v>10</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>13</v>
+        <v>141</v>
       </c>
       <c r="F20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1591,7 +1598,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21">
         <v>4</v>
@@ -1600,10 +1607,10 @@
         <v>10</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>13</v>
+        <v>141</v>
       </c>
       <c r="F21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1611,7 +1618,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22">
         <v>4</v>
@@ -1620,10 +1627,10 @@
         <v>10</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>13</v>
+        <v>141</v>
       </c>
       <c r="F22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1631,7 +1638,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C23">
         <v>4</v>
@@ -1640,10 +1647,10 @@
         <v>10</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>13</v>
+        <v>141</v>
       </c>
       <c r="F23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1651,7 +1658,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C24">
         <v>4</v>
@@ -1660,10 +1667,10 @@
         <v>10</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>13</v>
+        <v>141</v>
       </c>
       <c r="F24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1671,7 +1678,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C25">
         <v>4</v>
@@ -1680,10 +1687,10 @@
         <v>10</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>13</v>
+        <v>141</v>
       </c>
       <c r="F25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1735,7 +1742,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1750,7 +1757,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -1765,7 +1772,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -1780,7 +1787,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -1795,7 +1802,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
@@ -1810,7 +1817,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
@@ -1825,7 +1832,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D8" t="b">
         <v>0</v>
@@ -1840,7 +1847,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D9" t="b">
         <v>1</v>
@@ -1855,7 +1862,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D10" t="b">
         <v>0</v>
@@ -1870,7 +1877,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
@@ -1885,7 +1892,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
@@ -1900,7 +1907,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
@@ -1915,7 +1922,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D14" t="b">
         <v>0</v>
@@ -1930,7 +1937,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D15" t="b">
         <v>0</v>
@@ -1945,7 +1952,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D16" t="b">
         <v>1</v>
@@ -1960,7 +1967,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
@@ -1975,7 +1982,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D18" t="b">
         <v>1</v>
@@ -1990,7 +1997,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D19" t="b">
         <v>0</v>
@@ -2005,7 +2012,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D20" t="b">
         <v>0</v>
@@ -2020,7 +2027,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D21" t="b">
         <v>0</v>
@@ -2035,7 +2042,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D22" t="b">
         <v>0</v>
@@ -2050,7 +2057,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D23" t="b">
         <v>0</v>
@@ -2065,7 +2072,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D24" t="b">
         <v>0</v>
@@ -2080,7 +2087,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D25" t="b">
         <v>1</v>
@@ -2095,7 +2102,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D26" t="b">
         <v>0</v>
@@ -2110,7 +2117,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D27" t="b">
         <v>0</v>
@@ -2125,7 +2132,7 @@
         <v>27</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D28" t="b">
         <v>0</v>
@@ -2140,7 +2147,7 @@
         <v>28</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D29" t="b">
         <v>1</v>
@@ -2155,7 +2162,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D30" t="b">
         <v>0</v>
@@ -2170,7 +2177,7 @@
         <v>30</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D31" t="b">
         <v>0</v>
@@ -2185,7 +2192,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D32" t="b">
         <v>1</v>
@@ -2200,7 +2207,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D33" t="b">
         <v>0</v>
@@ -2215,7 +2222,7 @@
         <v>33</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D34" t="b">
         <v>0</v>
@@ -2230,7 +2237,7 @@
         <v>34</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D35" t="b">
         <v>1</v>
@@ -2245,7 +2252,7 @@
         <v>35</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D36" t="b">
         <v>0</v>
@@ -2260,7 +2267,7 @@
         <v>36</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D37" t="b">
         <v>0</v>
@@ -2275,7 +2282,7 @@
         <v>37</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D38" t="b">
         <v>0</v>
@@ -2290,7 +2297,7 @@
         <v>38</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D39" t="b">
         <v>0</v>
@@ -2305,7 +2312,7 @@
         <v>39</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D40" t="b">
         <v>0</v>
@@ -2320,7 +2327,7 @@
         <v>40</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D41" t="b">
         <v>1</v>
@@ -2335,7 +2342,7 @@
         <v>41</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D42" t="b">
         <v>0</v>
@@ -2350,7 +2357,7 @@
         <v>42</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D43" t="b">
         <v>1</v>
@@ -2365,7 +2372,7 @@
         <v>43</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D44" t="b">
         <v>0</v>
@@ -2380,7 +2387,7 @@
         <v>44</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D45" t="b">
         <v>0</v>
@@ -2395,7 +2402,7 @@
         <v>45</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D46" t="b">
         <v>0</v>
@@ -2410,7 +2417,7 @@
         <v>46</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D47" t="b">
         <v>0</v>
@@ -2425,7 +2432,7 @@
         <v>47</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D48" t="b">
         <v>1</v>
@@ -2440,7 +2447,7 @@
         <v>48</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D49" t="b">
         <v>0</v>
@@ -2455,7 +2462,7 @@
         <v>49</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D50" t="b">
         <v>0</v>
@@ -2470,7 +2477,7 @@
         <v>50</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D51" t="b">
         <v>1</v>
@@ -2485,7 +2492,7 @@
         <v>51</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D52" t="b">
         <v>0</v>
@@ -2500,7 +2507,7 @@
         <v>52</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D53" t="b">
         <v>0</v>
@@ -2515,7 +2522,7 @@
         <v>53</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D54" t="b">
         <v>1</v>
@@ -2530,7 +2537,7 @@
         <v>54</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D55" t="b">
         <v>0</v>
@@ -2545,7 +2552,7 @@
         <v>55</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D56" t="b">
         <v>0</v>
@@ -2560,7 +2567,7 @@
         <v>56</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D57" t="b">
         <v>0</v>
@@ -2575,7 +2582,7 @@
         <v>57</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D58" t="b">
         <v>0</v>
@@ -2590,7 +2597,7 @@
         <v>58</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D59" t="b">
         <v>0</v>
@@ -2605,7 +2612,7 @@
         <v>59</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D60" t="b">
         <v>0</v>
@@ -2620,7 +2627,7 @@
         <v>60</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D61" t="b">
         <v>1</v>
@@ -2650,7 +2657,7 @@
         <v>62</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D63" t="b">
         <v>0</v>
@@ -2680,7 +2687,7 @@
         <v>64</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D65" t="b">
         <v>0</v>
@@ -2695,7 +2702,7 @@
         <v>65</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D66" t="b">
         <v>1</v>
@@ -2710,7 +2717,7 @@
         <v>66</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D67" t="b">
         <v>0</v>
@@ -2725,7 +2732,7 @@
         <v>67</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D68" t="b">
         <v>0</v>
@@ -2740,7 +2747,7 @@
         <v>68</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D69" t="b">
         <v>0</v>
@@ -2755,7 +2762,7 @@
         <v>69</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D70" t="b">
         <v>1</v>
@@ -2770,7 +2777,7 @@
         <v>70</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D71" t="b">
         <v>0</v>
@@ -2785,7 +2792,7 @@
         <v>71</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D72" t="b">
         <v>0</v>
@@ -2800,7 +2807,7 @@
         <v>72</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D73" t="b">
         <v>0</v>
@@ -2815,7 +2822,7 @@
         <v>73</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D74" t="b">
         <v>1</v>
@@ -2830,7 +2837,7 @@
         <v>74</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D75" t="b">
         <v>0</v>
@@ -2845,7 +2852,7 @@
         <v>75</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D76" t="b">
         <v>0</v>
@@ -2860,7 +2867,7 @@
         <v>76</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D77" t="b">
         <v>0</v>
@@ -2875,7 +2882,7 @@
         <v>77</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D78" t="b">
         <v>0</v>
@@ -2890,7 +2897,7 @@
         <v>78</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D79" t="b">
         <v>1</v>
@@ -2905,7 +2912,7 @@
         <v>79</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D80" t="b">
         <v>0</v>
@@ -2920,7 +2927,7 @@
         <v>80</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D81" t="b">
         <v>0</v>
@@ -2935,7 +2942,7 @@
         <v>81</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D82" t="b">
         <v>0</v>
@@ -2950,7 +2957,7 @@
         <v>82</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D83" t="b">
         <v>1</v>
@@ -2965,7 +2972,7 @@
         <v>83</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D84" t="b">
         <v>0</v>
@@ -2980,7 +2987,7 @@
         <v>84</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D85" t="b">
         <v>0</v>
@@ -2995,7 +3002,7 @@
         <v>85</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D86" t="b">
         <v>1</v>
@@ -3010,7 +3017,7 @@
         <v>86</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D87" t="b">
         <v>0</v>
@@ -3025,7 +3032,7 @@
         <v>87</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D88" t="b">
         <v>0</v>
@@ -3040,7 +3047,7 @@
         <v>88</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D89" t="b">
         <v>0</v>
@@ -3055,7 +3062,7 @@
         <v>89</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D90" t="b">
         <v>1</v>
@@ -3070,7 +3077,7 @@
         <v>90</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D91" t="b">
         <v>0</v>
@@ -3085,7 +3092,7 @@
         <v>91</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D92" t="b">
         <v>0</v>
@@ -3100,7 +3107,7 @@
         <v>92</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D93" t="b">
         <v>0</v>
@@ -3115,7 +3122,7 @@
         <v>93</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D94" t="b">
         <v>0</v>
@@ -3130,7 +3137,7 @@
         <v>94</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D95" t="b">
         <v>1</v>
@@ -3145,7 +3152,7 @@
         <v>95</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D96" t="b">
         <v>0</v>
@@ -3160,7 +3167,7 @@
         <v>96</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D97" t="b">
         <v>0</v>
@@ -3175,7 +3182,7 @@
         <v>97</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D98" t="b">
         <v>0</v>
@@ -3190,7 +3197,7 @@
         <v>98</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D99" t="b">
         <v>0</v>
@@ -3205,7 +3212,7 @@
         <v>99</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D100" t="b">
         <v>0</v>
@@ -3220,7 +3227,7 @@
         <v>100</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D101" t="b">
         <v>1</v>

</xml_diff>